<commit_message>
Added passing test cases with justifications
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E5FD32-4D75-4CFB-8BE1-1F3509717B26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF0029C-2E57-4935-8FAE-8CEDE8CCDF08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="27634" windowHeight="15034" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Test Scenario: Portfolio Website</t>
   </si>
@@ -84,9 +84,6 @@
     <t>test_&lt;NavigateToComment&gt;</t>
   </si>
   <si>
-    <t>This is to test whether users are able to successfully navigate to a page to leave comments</t>
-  </si>
-  <si>
     <t>Navigated to page to comment</t>
   </si>
   <si>
@@ -94,6 +91,51 @@
   </si>
   <si>
     <t>Justification</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to successfully navigate to the blog pages to leave comments</t>
+  </si>
+  <si>
+    <t>test_&lt;NavigateToBlogPages&gt;</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to navigate to each blog pages</t>
+  </si>
+  <si>
+    <t>Navigated to each Blog pages</t>
+  </si>
+  <si>
+    <t>test_&lt;NavigateToProjectPages&gt;</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to navigate to each project pages</t>
+  </si>
+  <si>
+    <t>Navigated to each Project pages</t>
+  </si>
+  <si>
+    <t>test_&lt;ViewResume&gt;</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to view a created Resume</t>
+  </si>
+  <si>
+    <t>Resume page is shown</t>
+  </si>
+  <si>
+    <t>test_&lt;SelfIntro&gt;</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to view a created SelfIntro</t>
+  </si>
+  <si>
+    <t>Self Intro page is shown</t>
+  </si>
+  <si>
+    <t>Based on the given source code, this function has already been implemented</t>
+  </si>
+  <si>
+    <t>Based on the given source code, I created a blog post as a Resume in the /admin page</t>
   </si>
 </sst>
 </file>
@@ -145,13 +187,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,7 +508,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -512,7 +551,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
@@ -534,6 +573,9 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4">
@@ -554,6 +596,9 @@
       <c r="F4" t="s">
         <v>15</v>
       </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5">
@@ -563,37 +608,111 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
-        <v>19</v>
+      <c r="G5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Made changes to source code to include Hobbies and CCAs
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF0029C-2E57-4935-8FAE-8CEDE8CCDF08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9AE404-CB4E-4F2A-9273-FE5CF7CED239}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="27634" windowHeight="15034" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>Test Scenario: Portfolio Website</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Resume page is shown</t>
   </si>
   <si>
-    <t>test_&lt;SelfIntro&gt;</t>
-  </si>
-  <si>
     <t>This is to test whether users are able to view a created SelfIntro</t>
   </si>
   <si>
@@ -136,6 +133,27 @@
   </si>
   <si>
     <t>Based on the given source code, I created a blog post as a Resume in the /admin page</t>
+  </si>
+  <si>
+    <t>test_&lt;ViewSelfIntro&gt;</t>
+  </si>
+  <si>
+    <t>test_&lt;ViewHobbies&gt;</t>
+  </si>
+  <si>
+    <t>test_&lt;ViewCCA&gt;</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to view a list of hobbies</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to view a list of CCAs</t>
+  </si>
+  <si>
+    <t>Hobbies are shown</t>
+  </si>
+  <si>
+    <t>CCAs are shown</t>
   </si>
 </sst>
 </file>
@@ -508,7 +526,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -574,7 +592,7 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
@@ -597,7 +615,7 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -620,7 +638,7 @@
         <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -643,7 +661,7 @@
         <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
@@ -666,7 +684,7 @@
         <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
@@ -689,7 +707,7 @@
         <v>29</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
@@ -697,32 +715,56 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>32</v>
-      </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created displaying pytest test cases
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9AE404-CB4E-4F2A-9273-FE5CF7CED239}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AE2689-0E1B-45A2-B981-791EEE3232D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="27634" windowHeight="15034" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>Test Scenario: Portfolio Website</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>CCAs are shown</t>
+  </si>
+  <si>
+    <t>Changed source code</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -749,6 +752,12 @@
       <c r="E10" t="s">
         <v>39</v>
       </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11">
@@ -765,6 +774,12 @@
       </c>
       <c r="E11" t="s">
         <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added codes to pass test cases
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AE2689-0E1B-45A2-B981-791EEE3232D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBD6D30-DD1A-4DDA-B57E-981B483C177C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="27634" windowHeight="15034" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
+    <workbookView xWindow="2426" yWindow="3480" windowWidth="13345" windowHeight="10869" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -526,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B0045C-8C77-417C-A292-19ED30892C0C}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -782,6 +782,11 @@
         <v>41</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Added codes for comment test cases
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBD6D30-DD1A-4DDA-B57E-981B483C177C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF6F7D1-D8B5-473F-9ED5-1DB8D1039324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2426" yWindow="3480" windowWidth="13345" windowHeight="10869" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="27634" windowHeight="15034" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>Test Scenario: Portfolio Website</t>
   </si>
@@ -157,6 +157,31 @@
   </si>
   <si>
     <t>Changed source code</t>
+  </si>
+  <si>
+    <t>test_&lt;SubmitComment&gt;</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to submit a comment</t>
+  </si>
+  <si>
+    <t>Name = "John Low" 
+Comment = "Your Resume is interesting"</t>
+  </si>
+  <si>
+    <t>Comment is displayed under the 'Comments' secton in the blog page</t>
+  </si>
+  <si>
+    <t>test_&lt;SubmitEmptyComment&gt;</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to submit an empty comment</t>
+  </si>
+  <si>
+    <t>Error displayed. Require users to fill in the 2 textboxes</t>
+  </si>
+  <si>
+    <t>Not able to test this function in pytest because error is only displayed on client side</t>
   </si>
 </sst>
 </file>
@@ -208,10 +233,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B0045C-8C77-417C-A292-19ED30892C0C}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -782,9 +810,55 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test cases for admin page
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF6F7D1-D8B5-473F-9ED5-1DB8D1039324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A497E2B-A8F8-44C2-91D8-19D61C8078E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="27634" windowHeight="15034" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
   <si>
     <t>Test Scenario: Portfolio Website</t>
   </si>
@@ -182,6 +182,62 @@
   </si>
   <si>
     <t>Not able to test this function in pytest because error is only displayed on client side</t>
+  </si>
+  <si>
+    <t>Test Scenario: Portfolio Admin Site</t>
+  </si>
+  <si>
+    <t>test_CreateBlog</t>
+  </si>
+  <si>
+    <t>test_EditBlog</t>
+  </si>
+  <si>
+    <t>test_DeleteBlog</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to create a blog</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to delete a blog</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to edit a blog</t>
+  </si>
+  <si>
+    <t>Title: Interesting Facts
+Body: IT is the largest growing industry
+Categories: Category object (4)</t>
+  </si>
+  <si>
+    <t>test_createCategory</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to create a category</t>
+  </si>
+  <si>
+    <t>Name: Facts</t>
+  </si>
+  <si>
+    <t>The new category is created</t>
+  </si>
+  <si>
+    <t>The new blog is created</t>
+  </si>
+  <si>
+    <t>The blog is edited with new information</t>
+  </si>
+  <si>
+    <t>The blog is deleted</t>
+  </si>
+  <si>
+    <t>test_DeleteCategory</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to delete a category</t>
+  </si>
+  <si>
+    <t>The category is deleted</t>
   </si>
 </sst>
 </file>
@@ -233,13 +289,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B0045C-8C77-417C-A292-19ED30892C0C}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -861,6 +918,145 @@
         <v>12</v>
       </c>
     </row>
+    <row r="21" spans="1:7" ht="18.45" x14ac:dyDescent="0.5">
+      <c r="A21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A23" s="1"/>
+      <c r="B23" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Created codes for admin test cases
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A497E2B-A8F8-44C2-91D8-19D61C8078E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5FF6C1-6B45-4A17-B2C3-7FC04249BFB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="27634" windowHeight="15034" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
   <si>
     <t>Test Scenario: Portfolio Website</t>
   </si>
@@ -238,6 +238,18 @@
   </si>
   <si>
     <t>The category is deleted</t>
+  </si>
+  <si>
+    <t>test_&lt;LoadingSpeed&gt;</t>
+  </si>
+  <si>
+    <t>This is to test whether website is able to open in 4000ms</t>
+  </si>
+  <si>
+    <t>Opens in 4 seconds</t>
+  </si>
+  <si>
+    <t>Not able to test this function in pytest because loading of website using Selenium is inconsistent</t>
   </si>
 </sst>
 </file>
@@ -613,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B0045C-8C77-417C-A292-19ED30892C0C}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -917,6 +929,24 @@
       <c r="A14">
         <v>12</v>
       </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">
@@ -1038,6 +1068,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>4</v>
+      </c>
       <c r="B27" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
Wrote 'Create Project Object' test case
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5FF6C1-6B45-4A17-B2C3-7FC04249BFB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEF5729-0612-4C2A-AAB7-079F3593400B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="27634" windowHeight="15034" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
+    <workbookView xWindow="12540" yWindow="1509" windowWidth="13346" windowHeight="10868" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="76">
   <si>
     <t>Test Scenario: Portfolio Website</t>
   </si>
@@ -250,6 +250,21 @@
   </si>
   <si>
     <t>Not able to test this function in pytest because loading of website using Selenium is inconsistent</t>
+  </si>
+  <si>
+    <t>test_&lt;CreateProject&gt;</t>
+  </si>
+  <si>
+    <t>This is to test whether a project can be created successfully</t>
+  </si>
+  <si>
+    <t>title: "New Project"
+description: "Testing project"
+technology: "Project"
+image: "img/project1.png"</t>
+  </si>
+  <si>
+    <t>A project object is created</t>
   </si>
 </sst>
 </file>
@@ -625,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B0045C-8C77-417C-A292-19ED30892C0C}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -948,6 +963,23 @@
         <v>71</v>
       </c>
     </row>
+    <row r="15" spans="1:7" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="21" spans="1:7" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Added create user test case
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34C6712-A726-433F-BF1B-6B03D10AD6BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172833AD-E1EC-451D-8431-CE9B22E1ED2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12540" yWindow="1509" windowWidth="13346" windowHeight="10868" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="82">
   <si>
     <t>Test Scenario: Portfolio Website</t>
   </si>
@@ -268,6 +268,23 @@
   </si>
   <si>
     <t>Based on the given source code, project object can be created through command prompt</t>
+  </si>
+  <si>
+    <t>test_CreateUser</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to create a new user</t>
+  </si>
+  <si>
+    <t>Username: JohnnyDoe
+Password: JohnnyDoe@1
+Password confirmation: JohnnyDoe@1</t>
+  </si>
+  <si>
+    <t>A new user is created</t>
+  </si>
+  <si>
+    <t>Case failed</t>
   </si>
 </sst>
 </file>
@@ -641,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B0045C-8C77-417C-A292-19ED30892C0C}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="D17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1022,7 +1039,9 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
       <c r="B23" s="4" t="s">
         <v>58</v>
       </c>
@@ -1044,7 +1063,7 @@
     </row>
     <row r="24" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
         <v>51</v>
@@ -1067,7 +1086,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
         <v>52</v>
@@ -1087,7 +1106,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
         <v>53</v>
@@ -1110,7 +1129,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
         <v>65</v>
@@ -1129,6 +1148,26 @@
       </c>
       <c r="G27" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created test case code
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172833AD-E1EC-451D-8431-CE9B22E1ED2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B9705A-6797-44BC-9D79-D7969D7CC6B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12540" yWindow="1509" windowWidth="13346" windowHeight="10868" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
@@ -276,15 +276,15 @@
     <t>This is to test whether users are able to create a new user</t>
   </si>
   <si>
+    <t>A new user is created</t>
+  </si>
+  <si>
+    <t>Case failed</t>
+  </si>
+  <si>
     <t>Username: JohnnyDoe
-Password: JohnnyDoe@1
-Password confirmation: JohnnyDoe@1</t>
-  </si>
-  <si>
-    <t>A new user is created</t>
-  </si>
-  <si>
-    <t>Case failed</t>
+Password: DjangoProject@1
+Password confirmation: DjangoProject@1</t>
   </si>
 </sst>
 </file>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B0045C-8C77-417C-A292-19ED30892C0C}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1161,13 +1161,13 @@
         <v>78</v>
       </c>
       <c r="D28" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Passed CreateUser test case
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B9705A-6797-44BC-9D79-D7969D7CC6B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D8B98B-F33B-4EAD-9DF9-807C9E56697C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12540" yWindow="1509" windowWidth="13346" windowHeight="10868" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
+    <workbookView xWindow="1577" yWindow="2614" windowWidth="13346" windowHeight="10869" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="81">
   <si>
     <t>Test Scenario: Portfolio Website</t>
   </si>
@@ -277,9 +277,6 @@
   </si>
   <si>
     <t>A new user is created</t>
-  </si>
-  <si>
-    <t>Case failed</t>
   </si>
   <si>
     <t>Username: JohnnyDoe
@@ -660,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B0045C-8C77-417C-A292-19ED30892C0C}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="D17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1161,13 +1158,16 @@
         <v>78</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>79</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="G28" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created new deleteuser test case
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D8B98B-F33B-4EAD-9DF9-807C9E56697C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B9EB48-0E1E-4F61-B10F-3742EAFB9854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1577" yWindow="2614" windowWidth="13346" windowHeight="10869" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
   <si>
     <t>Test Scenario: Portfolio Website</t>
   </si>
@@ -282,6 +282,18 @@
     <t>Username: JohnnyDoe
 Password: DjangoProject@1
 Password confirmation: DjangoProject@1</t>
+  </si>
+  <si>
+    <t>test_DeleteUser</t>
+  </si>
+  <si>
+    <t>This is to test whether users are able to delete an existing user</t>
+  </si>
+  <si>
+    <t>User is deleteds</t>
+  </si>
+  <si>
+    <t>Case failed</t>
   </si>
 </sst>
 </file>
@@ -655,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B0045C-8C77-417C-A292-19ED30892C0C}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1170,6 +1182,26 @@
         <v>32</v>
       </c>
     </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Passed DeleteUser test case
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B9EB48-0E1E-4F61-B10F-3742EAFB9854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6751E225-9F4F-4B1E-AAA3-311F1864CA8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1577" yWindow="2614" windowWidth="13346" windowHeight="10869" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="84">
   <si>
     <t>Test Scenario: Portfolio Website</t>
   </si>
@@ -290,10 +290,7 @@
     <t>This is to test whether users are able to delete an existing user</t>
   </si>
   <si>
-    <t>User is deleteds</t>
-  </si>
-  <si>
-    <t>Case failed</t>
+    <t>User is deleted</t>
   </si>
 </sst>
 </file>
@@ -670,7 +667,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1199,7 +1196,10 @@
         <v>83</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="G29" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created test case for Read More Project
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6751E225-9F4F-4B1E-AAA3-311F1864CA8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF741663-E79F-4281-86FC-1B89BFAE0E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1577" yWindow="2614" windowWidth="13346" windowHeight="10869" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
+    <workbookView xWindow="13714" yWindow="0" windowWidth="13715" windowHeight="14829" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
   <si>
     <t>Test Scenario: Portfolio Website</t>
   </si>
@@ -129,12 +129,6 @@
     <t>Self Intro page is shown</t>
   </si>
   <si>
-    <t>Based on the given source code, this function has already been implemented</t>
-  </si>
-  <si>
-    <t>Based on the given source code, I created a blog post as a Resume in the /admin page</t>
-  </si>
-  <si>
     <t>test_&lt;ViewSelfIntro&gt;</t>
   </si>
   <si>
@@ -154,9 +148,6 @@
   </si>
   <si>
     <t>CCAs are shown</t>
-  </si>
-  <si>
-    <t>Changed source code</t>
   </si>
   <si>
     <t>test_&lt;SubmitComment&gt;</t>
@@ -267,9 +258,6 @@
     <t>A project object is created</t>
   </si>
   <si>
-    <t>Based on the given source code, project object can be created through command prompt</t>
-  </si>
-  <si>
     <t>test_CreateUser</t>
   </si>
   <si>
@@ -291,6 +279,24 @@
   </si>
   <si>
     <t>User is deleted</t>
+  </si>
+  <si>
+    <t>Passed test case</t>
+  </si>
+  <si>
+    <t>Not able to test this function, but based on the given source code, project object can be created through command prompt</t>
+  </si>
+  <si>
+    <t>test_&lt;ReadMorePortfolio&gt;</t>
+  </si>
+  <si>
+    <t>This is to test whether users can click on 'Read More' to display project details</t>
+  </si>
+  <si>
+    <t>Project details displayed</t>
+  </si>
+  <si>
+    <t>Failed test case</t>
   </si>
 </sst>
 </file>
@@ -666,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B0045C-8C77-417C-A292-19ED30892C0C}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -733,7 +739,7 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
@@ -756,7 +762,7 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -779,7 +785,7 @@
         <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -802,7 +808,7 @@
         <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
@@ -825,7 +831,7 @@
         <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
@@ -848,7 +854,7 @@
         <v>29</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
@@ -856,7 +862,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
@@ -871,7 +877,7 @@
         <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
@@ -879,22 +885,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
-      </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
@@ -902,22 +908,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
         <v>36</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
         <v>38</v>
       </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
@@ -925,22 +931,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
         <v>42</v>
       </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" t="s">
-        <v>45</v>
-      </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
@@ -948,22 +954,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" t="s">
         <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
@@ -971,22 +977,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
         <v>68</v>
-      </c>
-      <c r="C14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="58.3" x14ac:dyDescent="0.4">
@@ -994,27 +1000,47 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" t="s">
         <v>72</v>
       </c>
-      <c r="C15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" t="s">
-        <v>75</v>
-      </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
@@ -1049,22 +1075,22 @@
         <v>1</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C23" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="F23" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G23" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
@@ -1072,22 +1098,22 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
         <v>51</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="E24" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G24" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
@@ -1095,19 +1121,19 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G25" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
@@ -1115,22 +1141,22 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G26" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
@@ -1138,22 +1164,22 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G27" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
@@ -1161,22 +1187,22 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G28" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.4">
@@ -1184,22 +1210,22 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G29" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created codes for test case ReadMoreProject
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF741663-E79F-4281-86FC-1B89BFAE0E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8541BD43-336F-4294-A5B0-9B58EB5D4CDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13714" yWindow="0" windowWidth="13715" windowHeight="14829" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="85">
   <si>
     <t>Test Scenario: Portfolio Website</t>
   </si>
@@ -294,9 +294,6 @@
   </si>
   <si>
     <t>Project details displayed</t>
-  </si>
-  <si>
-    <t>Failed test case</t>
   </si>
 </sst>
 </file>
@@ -673,7 +670,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F16" sqref="F16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1034,9 +1031,6 @@
       <c r="E16" t="s">
         <v>84</v>
       </c>
-      <c r="G16" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="21" spans="1:7" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">

</xml_diff>

<commit_message>
Test case ReadMoreProject Passed
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ng Hsiao Jiet\ETI-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8541BD43-336F-4294-A5B0-9B58EB5D4CDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292C5E61-0049-434A-BA06-C2BB115A2CA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13714" yWindow="0" windowWidth="13715" windowHeight="14829" xr2:uid="{F725CD1C-1319-4DF0-8ADF-3EFFFB58E3BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="85">
   <si>
     <t>Test Scenario: Portfolio Website</t>
   </si>
@@ -670,7 +670,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:G16"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1031,6 +1031,12 @@
       <c r="E16" t="s">
         <v>84</v>
       </c>
+      <c r="F16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">

</xml_diff>